<commit_message>
Version 9.3 Fixed Player ratings
</commit_message>
<xml_diff>
--- a/player_ratings_data.xlsx
+++ b/player_ratings_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\OpenMatchEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6294CAD5-3F83-404B-999A-ED1F9FC1BCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F39F2DD-17F8-4677-A16E-95481379A31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5025" yWindow="5025" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -685,11 +685,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -954,10 +957,10 @@
         <v>56</v>
       </c>
       <c r="B4">
-        <v>-560</v>
+        <v>-540</v>
       </c>
       <c r="C4">
-        <v>-720</v>
+        <v>-700</v>
       </c>
       <c r="D4">
         <v>-680</v>
@@ -1556,85 +1559,85 @@
         <v>63</v>
       </c>
       <c r="B11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="C11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="D11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="F11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="G11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="H11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="I11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="K11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="L11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="M11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="N11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="O11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="P11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Q11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="R11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="S11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="T11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="U11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="V11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="W11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="X11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Y11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Z11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AA11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AB11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -2244,85 +2247,85 @@
         <v>71</v>
       </c>
       <c r="B19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="C19">
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="D19">
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="E19">
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="F19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="G19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="H19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="I19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="J19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="K19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="L19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="M19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="N19">
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="O19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="P19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="Q19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="R19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="S19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="T19">
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="U19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="V19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="W19">
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="X19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="Y19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="Z19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="AA19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="AB19">
-        <v>-18</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -2846,22 +2849,22 @@
         <v>78</v>
       </c>
       <c r="B26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="C26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="D26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E26">
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="G26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="H26">
         <v>10</v>
@@ -2879,10 +2882,10 @@
         <v>10</v>
       </c>
       <c r="M26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="N26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="O26">
         <v>10</v>
@@ -2900,7 +2903,7 @@
         <v>10</v>
       </c>
       <c r="T26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="U26">
         <v>10</v>
@@ -2909,7 +2912,7 @@
         <v>10</v>
       </c>
       <c r="W26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="X26">
         <v>10</v>
@@ -2918,13 +2921,13 @@
         <v>10</v>
       </c>
       <c r="Z26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="AA26">
         <v>10</v>
       </c>
       <c r="AB26">
-        <v>-50</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
@@ -3964,7 +3967,7 @@
         <v>91</v>
       </c>
       <c r="B39">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C39">
         <v>2</v>

</xml_diff>

<commit_message>
Version 9.4 Totally last fix to player ratings decoding
</commit_message>
<xml_diff>
--- a/player_ratings_data.xlsx
+++ b/player_ratings_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\OpenMatchEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F39F2DD-17F8-4677-A16E-95481379A31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56E5C0A-FC29-472E-BA71-CEA376861690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="5025" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="2925" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -685,14 +685,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -957,13 +954,13 @@
         <v>56</v>
       </c>
       <c r="B4">
-        <v>-540</v>
+        <v>-560</v>
       </c>
       <c r="C4">
+        <v>-770</v>
+      </c>
+      <c r="D4">
         <v>-700</v>
-      </c>
-      <c r="D4">
-        <v>-680</v>
       </c>
       <c r="E4">
         <v>-780</v>
@@ -1559,85 +1556,85 @@
         <v>63</v>
       </c>
       <c r="B11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="I11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="J11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="K11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="L11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="M11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="N11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="O11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="P11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="Q11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="R11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="S11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="T11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="U11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="V11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="W11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="X11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="Y11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="Z11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="AA11">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="AB11">
-        <v>-3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -2247,85 +2244,85 @@
         <v>71</v>
       </c>
       <c r="B19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>-19</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>-19</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>-19</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="H19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="I19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="J19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="K19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="L19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="M19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="N19">
-        <v>-19</v>
+        <v>5</v>
       </c>
       <c r="O19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="P19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="Q19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="R19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="S19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="T19">
-        <v>-19</v>
+        <v>5</v>
       </c>
       <c r="U19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="V19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="W19">
-        <v>-19</v>
+        <v>5</v>
       </c>
       <c r="X19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="Y19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="Z19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="AA19">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="AB19">
-        <v>-19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -2333,7 +2330,7 @@
         <v>72</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>-15</v>
@@ -2366,7 +2363,7 @@
         <v>-14</v>
       </c>
       <c r="M20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N20">
         <v>-15</v>
@@ -2763,85 +2760,85 @@
         <v>77</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB25">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
@@ -2849,22 +2846,22 @@
         <v>78</v>
       </c>
       <c r="B26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>10</v>
       </c>
       <c r="F26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="H26">
         <v>10</v>
@@ -2882,10 +2879,10 @@
         <v>10</v>
       </c>
       <c r="M26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="N26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="O26">
         <v>10</v>
@@ -2903,7 +2900,7 @@
         <v>10</v>
       </c>
       <c r="T26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="U26">
         <v>10</v>
@@ -2912,7 +2909,7 @@
         <v>10</v>
       </c>
       <c r="W26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="X26">
         <v>10</v>
@@ -2921,13 +2918,13 @@
         <v>10</v>
       </c>
       <c r="Z26">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="AA26">
         <v>10</v>
       </c>
       <c r="AB26">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
@@ -3365,7 +3362,7 @@
         <v>84</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>30</v>
@@ -3398,7 +3395,7 @@
         <v>10</v>
       </c>
       <c r="M32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N32">
         <v>30</v>
@@ -3537,7 +3534,7 @@
         <v>86</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <v>10</v>
@@ -3570,7 +3567,7 @@
         <v>10</v>
       </c>
       <c r="M34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N34">
         <v>10</v>
@@ -3967,85 +3964,85 @@
         <v>91</v>
       </c>
       <c r="B39">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M39">
         <v>100</v>
       </c>
       <c r="N39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB39">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -4056,82 +4053,82 @@
         <v>200</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M40">
         <v>200</v>
       </c>
       <c r="N40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB40">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
@@ -4142,82 +4139,82 @@
         <v>400</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M41">
         <v>400</v>
       </c>
       <c r="N41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB41">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
@@ -4228,82 +4225,82 @@
         <v>450</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M42">
         <v>450</v>
       </c>
       <c r="N42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB42">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
@@ -4311,85 +4308,85 @@
         <v>95</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB43">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
@@ -4400,82 +4397,82 @@
         <v>125</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M44">
         <v>125</v>
       </c>
       <c r="N44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB44">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.25">
@@ -4916,82 +4913,82 @@
         <v>300</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M50">
         <v>300</v>
       </c>
       <c r="N50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB50">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.25">
@@ -5088,82 +5085,82 @@
         <v>300</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M52">
         <v>300</v>
       </c>
       <c r="N52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB52">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Version 0.9.5 - Updated weights
</commit_message>
<xml_diff>
--- a/player_ratings_data.xlsx
+++ b/player_ratings_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\OpenMatchEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56E5C0A-FC29-472E-BA71-CEA376861690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997A30AF-BC19-4246-B08D-E8F34125C0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="2925" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,7 +686,7 @@
   <dimension ref="A1:AB55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,13 +957,13 @@
         <v>-560</v>
       </c>
       <c r="C4">
-        <v>-770</v>
+        <v>-700</v>
       </c>
       <c r="D4">
-        <v>-700</v>
+        <v>-670</v>
       </c>
       <c r="E4">
-        <v>-780</v>
+        <v>-730</v>
       </c>
       <c r="F4">
         <v>-650</v>

</xml_diff>